<commit_message>
update in room rents wel come
</commit_message>
<xml_diff>
--- a/ROOM  RENTS.xlsx
+++ b/ROOM  RENTS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="RENTS" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="java" sheetId="7" r:id="rId7"/>
     <sheet name="WINDOWS" sheetId="8" r:id="rId8"/>
     <sheet name="MARC AND APR 23" sheetId="9" r:id="rId9"/>
+    <sheet name="git start 1002023" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
   <si>
     <t>GOPI</t>
   </si>
@@ -328,6 +329,9 @@
   </si>
   <si>
     <t>CLEAR ON 31MAY23</t>
+  </si>
+  <si>
+    <t>wel come to gi hub</t>
   </si>
 </sst>
 </file>
@@ -1506,6 +1510,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E2:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:6">
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6">
+      <c r="F4" s="38">
+        <v>45078</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:N23"/>
@@ -3101,7 +3133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>